<commit_message>
unittest database with indexes on some fields
</commit_message>
<xml_diff>
--- a/database/xlsx/unittest.xlsx
+++ b/database/xlsx/unittest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="91">
   <si>
     <t>Database: Unit Test</t>
   </si>
@@ -64,6 +64,9 @@
     <t>Field Name</t>
   </si>
   <si>
+    <t>Index</t>
+  </si>
+  <si>
     <t>Data Type</t>
   </si>
   <si>
@@ -73,7 +76,10 @@
     <t># Common fields list</t>
   </si>
   <si>
-    <t>RecID**</t>
+    <t>RecID</t>
+  </si>
+  <si>
+    <t>**</t>
   </si>
   <si>
     <t>uuid</t>
@@ -83,6 +89,9 @@
   </si>
   <si>
     <t>InsertTime</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
   <si>
     <t>timestamp</t>
@@ -284,7 +293,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="17">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -323,9 +332,6 @@
       <name val="&quot;Arial&quot;"/>
     </font>
     <font>
-      <sz val="12.0"/>
-    </font>
-    <font>
       <b/>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
@@ -334,29 +340,14 @@
     <font>
       <b/>
       <sz val="11.0"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12.0"/>
-    </font>
-    <font/>
     <font>
       <b/>
       <color theme="1"/>
@@ -413,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -456,9 +447,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -474,7 +462,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -486,48 +474,35 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -756,7 +731,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="58.86"/>
+    <col customWidth="1" min="1" max="1" width="45.71"/>
     <col customWidth="1" min="2" max="2" width="47.57"/>
     <col customWidth="1" min="3" max="3" width="47.86"/>
   </cols>
@@ -878,7 +853,7 @@
       <c r="D16" s="5"/>
     </row>
     <row r="17">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="16" t="s">
@@ -888,7 +863,7 @@
       <c r="D17" s="5"/>
     </row>
     <row r="18">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="16" t="s">
@@ -898,7 +873,7 @@
       <c r="D18" s="5"/>
     </row>
     <row r="19">
-      <c r="A19" s="19"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="5"/>
@@ -910,7 +885,7 @@
       <c r="D20" s="5"/>
     </row>
     <row r="21">
-      <c r="A21" s="20"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="5"/>
@@ -970,7 +945,7 @@
       <c r="D30" s="5"/>
     </row>
     <row r="31">
-      <c r="A31" s="21"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1018,25 +993,25 @@
       <c r="D38" s="5"/>
     </row>
     <row r="39">
-      <c r="A39" s="22"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
     </row>
     <row r="40">
-      <c r="A40" s="22"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
     </row>
     <row r="41">
-      <c r="A41" s="22"/>
+      <c r="A41" s="21"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
     </row>
     <row r="42">
-      <c r="A42" s="23"/>
+      <c r="A42" s="22"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1054,583 +1029,692 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="32.57"/>
-    <col customWidth="1" min="3" max="3" width="32.86"/>
-    <col customWidth="1" min="4" max="4" width="51.57"/>
-    <col customWidth="1" min="5" max="5" width="36.71"/>
+    <col customWidth="1" min="2" max="2" width="14.43"/>
+    <col customWidth="1" min="4" max="4" width="32.86"/>
+    <col customWidth="1" min="5" max="5" width="51.57"/>
+    <col customWidth="1" min="6" max="6" width="36.71"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="5"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
       <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="A3" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4">
-      <c r="A4" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="31" t="s">
+      <c r="A4" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="B4" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="C4" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>23</v>
+      </c>
       <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="5"/>
+      <c r="A5" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="25"/>
       <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="5"/>
+      <c r="A6" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="25"/>
       <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7">
-      <c r="A7" s="33"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8">
-      <c r="A8" s="33"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="25"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
+      <c r="A9" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
     </row>
     <row r="10">
-      <c r="A10" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="5"/>
+      <c r="A10" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>30</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="25"/>
       <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12">
-      <c r="A12" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="5"/>
+      <c r="A12" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13">
-      <c r="A13" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="5"/>
+      <c r="A13" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="25"/>
       <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14">
-      <c r="A14" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="5"/>
+      <c r="A14" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="25"/>
       <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15">
-      <c r="A15" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="5"/>
+      <c r="A15" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>39</v>
+      </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16">
-      <c r="A16" s="33"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="5"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17">
-      <c r="A17" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
+      <c r="A17" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
     </row>
     <row r="18">
-      <c r="A18" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="5"/>
+      <c r="A18" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19">
-      <c r="A19" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="5"/>
+      <c r="A19" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>36</v>
+      </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20">
-      <c r="A20" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="5"/>
+      <c r="A20" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="25"/>
       <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21">
-      <c r="A21" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="5"/>
+      <c r="A21" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="25"/>
       <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22">
-      <c r="A22" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="5"/>
+      <c r="A22" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="33"/>
+      <c r="C22" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="25"/>
       <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23">
-      <c r="A23" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="5"/>
+      <c r="A23" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="33"/>
+      <c r="C23" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="25"/>
       <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
     </row>
     <row r="24">
-      <c r="A24" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="5"/>
+      <c r="A24" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="33"/>
+      <c r="C24" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="25"/>
       <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25">
-      <c r="A25" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="5"/>
+      <c r="A25" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="33"/>
+      <c r="C25" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="25"/>
       <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26">
-      <c r="A26" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="5"/>
+      <c r="A26" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="33"/>
+      <c r="C26" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="25"/>
       <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27">
-      <c r="A27" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="5"/>
+      <c r="A27" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="25"/>
       <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28">
-      <c r="A28" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="5"/>
+      <c r="A28" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="33"/>
+      <c r="C28" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="25"/>
       <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
     </row>
     <row r="29">
-      <c r="A29" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="5"/>
+      <c r="A29" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="33"/>
+      <c r="C29" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="25"/>
       <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30">
-      <c r="A30" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="5"/>
+      <c r="A30" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="33"/>
+      <c r="C30" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="25"/>
       <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31">
-      <c r="A31" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="35" t="s">
-        <v>33</v>
+      <c r="A31" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="33"/>
+      <c r="C31" s="34" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="35" t="s">
-        <v>33</v>
+      <c r="A32" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="33"/>
+      <c r="C32" s="34" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="35" t="s">
-        <v>33</v>
+      <c r="A33" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="33"/>
+      <c r="C33" s="34" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>33</v>
+      <c r="A34" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="33"/>
+      <c r="C34" s="30" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" s="35" t="s">
-        <v>33</v>
+      <c r="A35" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="33"/>
+      <c r="C35" s="34" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" s="35" t="s">
-        <v>33</v>
+      <c r="A36" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="33"/>
+      <c r="C36" s="34" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" s="35" t="s">
-        <v>33</v>
+      <c r="A37" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="33"/>
+      <c r="C37" s="34" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="36"/>
-      <c r="B38" s="37"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="36"/>
     </row>
     <row r="39">
-      <c r="A39" s="36"/>
-      <c r="B39" s="37"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="36"/>
     </row>
     <row r="40">
-      <c r="A40" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" s="39"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
+      <c r="A40" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="26"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
     </row>
     <row r="41">
-      <c r="A41" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="40" t="s">
-        <v>27</v>
+      <c r="A41" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="41" t="s">
-        <v>27</v>
+      <c r="A42" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="37" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="41" t="s">
-        <v>27</v>
+      <c r="A43" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="37" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="40" t="s">
-        <v>27</v>
+      <c r="A44" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="41" t="s">
-        <v>27</v>
+      <c r="A45" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="41" t="s">
-        <v>27</v>
+      <c r="A46" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="B47" s="40" t="s">
-        <v>27</v>
+      <c r="A47" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="B48" s="41" t="s">
-        <v>27</v>
+      <c r="A48" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B49" s="41" t="s">
-        <v>27</v>
+      <c r="A49" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="B50" s="41" t="s">
-        <v>27</v>
+      <c r="A50" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="37"/>
-      <c r="B51" s="37"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
     </row>
     <row r="52">
-      <c r="A52" s="37"/>
-      <c r="B52" s="37"/>
+      <c r="A52" s="36"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
     </row>
     <row r="53">
-      <c r="A53" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="B53" s="39"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
+      <c r="A53" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" s="26"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
     </row>
     <row r="54">
-      <c r="A54" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="B54" s="40" t="s">
-        <v>36</v>
+      <c r="A54" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B54" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="B55" s="40" t="s">
-        <v>36</v>
+      <c r="A55" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="B56" s="40" t="s">
-        <v>36</v>
+      <c r="A56" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="B57" s="40" t="s">
-        <v>36</v>
+      <c r="A57" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="B58" s="40" t="s">
-        <v>36</v>
+      <c r="A58" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="B59" s="40" t="s">
-        <v>36</v>
+      <c r="A59" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="B60" s="40" t="s">
-        <v>36</v>
+      <c r="A60" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" s="37"/>
+      <c r="C60" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="B61" s="40" t="s">
-        <v>36</v>
+      <c r="A61" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="B62" s="40" t="s">
-        <v>36</v>
+      <c r="A62" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="B63" s="40" t="s">
-        <v>36</v>
+      <c r="A63" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="38"/>
-      <c r="B66" s="28"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29"/>
+      <c r="A66" s="26"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1648,140 +1732,164 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="29.29"/>
-    <col customWidth="1" min="2" max="2" width="18.57"/>
-    <col customWidth="1" min="3" max="3" width="36.86"/>
-    <col customWidth="1" min="4" max="4" width="37.71"/>
-    <col customWidth="1" min="5" max="5" width="32.0"/>
+    <col customWidth="1" min="2" max="2" width="11.43"/>
+    <col customWidth="1" min="3" max="3" width="18.57"/>
+    <col customWidth="1" min="4" max="4" width="36.86"/>
+    <col customWidth="1" min="5" max="5" width="37.71"/>
+    <col customWidth="1" min="6" max="6" width="32.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="A3" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
+      <c r="A6" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
     </row>
     <row r="7">
-      <c r="A7" s="43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="5"/>
+      <c r="A7" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>39</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8">
-      <c r="A8" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="5"/>
+      <c r="A8" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>39</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="44" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="5"/>
+      <c r="A9" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>39</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="46"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="46"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12">
-      <c r="A12" s="46"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13">
-      <c r="A13" s="46"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14">
-      <c r="A14" s="46"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15">
-      <c r="A15" s="47"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="41"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1799,155 +1907,183 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="33.0"/>
-    <col customWidth="1" min="2" max="2" width="25.43"/>
-    <col customWidth="1" min="3" max="3" width="23.57"/>
-    <col customWidth="1" min="4" max="4" width="31.0"/>
+    <col customWidth="1" min="2" max="2" width="20.43"/>
+    <col customWidth="1" min="3" max="3" width="25.43"/>
+    <col customWidth="1" min="4" max="4" width="23.57"/>
+    <col customWidth="1" min="5" max="5" width="31.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="A3" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5">
-      <c r="A5" s="26"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6">
-      <c r="A6" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
+      <c r="A6" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
     </row>
     <row r="7">
-      <c r="A7" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="5"/>
+      <c r="A7" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>39</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8">
-      <c r="A8" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="B8" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="5"/>
+      <c r="A8" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>39</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="5"/>
+      <c r="A9" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>39</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="33"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11">
-      <c r="A11" s="46"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12">
-      <c r="A12" s="46"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13">
-      <c r="A13" s="46"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14">
-      <c r="A14" s="46"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15">
-      <c r="A15" s="46"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16">
-      <c r="A16" s="47"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
     </row>
     <row r="17">
-      <c r="A17" s="47"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="41"/>
     </row>
     <row r="18">
-      <c r="A18" s="47"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
     </row>
     <row r="19">
-      <c r="A19" s="47"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>